<commit_message>
pase todo al informe, falta completar cositas y el emparrillado
</commit_message>
<xml_diff>
--- a/Terminos/Emparrillado.xlsx
+++ b/Terminos/Emparrillado.xlsx
@@ -16,43 +16,43 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="13">
   <si>
-    <t>Elemento 1</t>
-  </si>
-  <si>
-    <t>Elemento 2</t>
-  </si>
-  <si>
-    <t>Elemento 3</t>
-  </si>
-  <si>
-    <t>Elemento 4</t>
-  </si>
-  <si>
-    <t>Elemento 5</t>
-  </si>
-  <si>
-    <t>Elemento 6</t>
-  </si>
-  <si>
-    <t>Caracteristica 1</t>
-  </si>
-  <si>
-    <t>Caracteristica 2</t>
-  </si>
-  <si>
-    <t>Caracteristica 3</t>
-  </si>
-  <si>
-    <t>Caracteristica 4</t>
-  </si>
-  <si>
-    <t>Caracteristica 5</t>
-  </si>
-  <si>
-    <t>Caracteristica 6</t>
-  </si>
-  <si>
     <t>valor</t>
+  </si>
+  <si>
+    <t>Fastball</t>
+  </si>
+  <si>
+    <t>Riseball</t>
+  </si>
+  <si>
+    <t>Dropball</t>
+  </si>
+  <si>
+    <t>Curveball</t>
+  </si>
+  <si>
+    <t>ChangeUp</t>
+  </si>
+  <si>
+    <t>Screwball</t>
+  </si>
+  <si>
+    <t>Velocidad</t>
+  </si>
+  <si>
+    <t>Posición Cuerpo</t>
+  </si>
+  <si>
+    <t>Traza</t>
+  </si>
+  <si>
+    <t>Dirección</t>
+  </si>
+  <si>
+    <t>Efecto</t>
+  </si>
+  <si>
+    <t>Agarre</t>
   </si>
 </sst>
 </file>
@@ -627,7 +627,7 @@
   <dimension ref="A2:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -639,160 +639,160 @@
     <row r="3" spans="1:7" ht="15.75" thickBot="1">
       <c r="A3" s="13"/>
       <c r="B3" s="14" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1">
       <c r="A9" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>